<commit_message>
Update - add some more fields and fix bugs
</commit_message>
<xml_diff>
--- a/api/_files/otaAndEnrolmentSheet.xlsx
+++ b/api/_files/otaAndEnrolmentSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="OTA" sheetId="1" state="visible" r:id="rId2"/>
@@ -1000,8 +1000,8 @@
   </sheetPr>
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1014,7 +1014,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.6"/>
   </cols>
   <sheetData>
@@ -1250,7 +1250,7 @@
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
     </row>
-    <row r="17" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="27"/>
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
@@ -1741,20 +1741,20 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="53" width="27.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="53" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="53" width="47.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update - minor spreadsheet reorg and update fields
</commit_message>
<xml_diff>
--- a/api/_files/otaAndEnrolmentSheet.xlsx
+++ b/api/_files/otaAndEnrolmentSheet.xlsx
@@ -107,6 +107,9 @@
     <t xml:space="preserve">Finish</t>
   </si>
   <si>
+    <t xml:space="preserve">Is there any tailoring or customisation of the course required?</t>
+  </si>
+  <si>
     <t xml:space="preserve">VENUE DETAILS</t>
   </si>
   <si>
@@ -175,9 +178,6 @@
   </si>
   <si>
     <t xml:space="preserve">Department being trained? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there any tailoring or customisation of the course required?</t>
   </si>
   <si>
     <t xml:space="preserve">TRAINING RESOURCES</t>
@@ -760,6 +760,14 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -811,14 +819,6 @@
     <xf numFmtId="164" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -1001,10 +1001,10 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.43"/>
@@ -1014,7 +1014,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.6"/>
   </cols>
   <sheetData>
@@ -1267,140 +1267,140 @@
       <c r="J17" s="30"/>
     </row>
     <row r="18" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+    </row>
+    <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-    </row>
-    <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18" t="s">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="22" t="s">
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+    </row>
+    <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="33" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="F23" s="22"/>
+      <c r="G23" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-    </row>
-    <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="35" t="s">
+      <c r="H23" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-    </row>
-    <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="23" t="s">
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+    </row>
+    <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+    </row>
+    <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-    </row>
-    <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-    </row>
-    <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="37" t="s">
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="38"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
       <c r="E27" s="38"/>
       <c r="F27" s="38"/>
       <c r="G27" s="38"/>
@@ -1423,42 +1423,40 @@
       <c r="J28" s="39"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="40" t="s">
-        <v>34</v>
-      </c>
+      <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="40"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="34"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
+      <c r="A30" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
     </row>
     <row r="31" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
       <c r="E31" s="43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F31" s="43"/>
       <c r="G31" s="43"/>
@@ -1467,36 +1465,38 @@
       <c r="J31" s="43"/>
     </row>
     <row r="32" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
     </row>
     <row r="33" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="44"/>
       <c r="C33" s="44"/>
       <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
+      <c r="E33" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
     </row>
     <row r="34" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="38"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
       <c r="E34" s="38"/>
       <c r="F34" s="38"/>
       <c r="G34" s="38"/>
@@ -1505,30 +1505,30 @@
       <c r="J34" s="38"/>
     </row>
     <row r="35" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
     </row>
     <row r="36" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="45"/>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
     </row>
     <row r="37" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="13" t="s">
@@ -1545,20 +1545,20 @@
       <c r="J37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="41" t="s">
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
     </row>
     <row r="39" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="16"/>
@@ -1571,8 +1571,8 @@
       <c r="F39" s="46"/>
       <c r="G39" s="46"/>
       <c r="H39" s="46"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
     </row>
     <row r="40" customFormat="false" ht="31.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="47" t="s">
@@ -1592,7 +1592,7 @@
       <c r="I40" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="J40" s="36"/>
+      <c r="J40" s="38"/>
     </row>
     <row r="41" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="47" t="s">
@@ -1606,7 +1606,7 @@
       <c r="G41" s="47"/>
       <c r="H41" s="47"/>
       <c r="I41" s="47"/>
-      <c r="J41" s="36"/>
+      <c r="J41" s="38"/>
     </row>
     <row r="42" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="48" t="s">
@@ -1677,35 +1677,35 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="A18:J18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A20:J20"/>
     <mergeCell ref="A21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="A22:D23"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="H23:J23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A24:D25"/>
+    <mergeCell ref="E24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="E27:J27"/>
     <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="A31:D31"/>
     <mergeCell ref="E31:J31"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="E32:J32"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="E34:J34"/>
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="A36:J36"/>
     <mergeCell ref="A37:J37"/>

</xml_diff>

<commit_message>
UPDATE + REMOVE - correct spreadsheet locations and delete redundant rows
</commit_message>
<xml_diff>
--- a/api/_files/otaAndEnrolmentSheet.xlsx
+++ b/api/_files/otaAndEnrolmentSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t xml:space="preserve">Please complete and return as soon as possible</t>
   </si>
@@ -163,18 +163,6 @@
   </si>
   <si>
     <t xml:space="preserve">TRAINING SESSION DETAILS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you have a Mailbox Limit?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you have an existing archiving policy?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What mobile devices are in use?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any CRM or Workload Management system?</t>
   </si>
   <si>
     <t xml:space="preserve">Department being trained? </t>
@@ -635,7 +623,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="69">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -809,14 +797,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -998,10 +978,10 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1014,7 +994,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.6"/>
   </cols>
   <sheetData>
@@ -1449,200 +1429,144 @@
       <c r="J30" s="41"/>
     </row>
     <row r="31" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="43" t="s">
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+    </row>
+    <row r="32" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+    </row>
+    <row r="33" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-    </row>
-    <row r="32" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-    </row>
-    <row r="33" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="44" t="s">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+    </row>
+    <row r="34" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="45" t="s">
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-    </row>
-    <row r="34" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
     </row>
     <row r="35" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-    </row>
-    <row r="36" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="40"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+    </row>
+    <row r="36" customFormat="false" ht="31.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="45"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="24"/>
+      <c r="F36" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="28"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="J36" s="38"/>
     </row>
     <row r="37" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
+      <c r="A37" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="38"/>
     </row>
     <row r="38" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
+      <c r="A38" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="48"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
     </row>
     <row r="39" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="38"/>
-    </row>
-    <row r="40" customFormat="false" ht="31.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" s="24"/>
-      <c r="F40" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="G40" s="28"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="J40" s="38"/>
-    </row>
-    <row r="41" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="47" t="s">
+      <c r="A39" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="38"/>
-    </row>
-    <row r="42" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="49"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" s="50"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-    </row>
-    <row r="43" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="52"/>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
-    </row>
-    <row r="44" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+    </row>
+    <row r="40" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="80">
+  <mergeCells count="72">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
@@ -1698,31 +1622,23 @@
     <mergeCell ref="A28:J28"/>
     <mergeCell ref="A29:J29"/>
     <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A32:J32"/>
+    <mergeCell ref="A33:J33"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="E34:J34"/>
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="A37:J37"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="F43:J43"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="F39:J39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1748,9 +1664,9 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="53" width="27.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="53" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="53" width="47.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="51" width="27.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="51" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="51" width="47.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.71"/>
@@ -1758,75 +1674,75 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="57"/>
+    </row>
+    <row r="2" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="57" t="s">
+      <c r="H2" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="59"/>
-    </row>
-    <row r="2" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="60" t="s">
+      <c r="I2" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="61" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="63"/>
+      <c r="B3" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="C3" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="63" t="s">
+      <c r="D3" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="E3" s="64" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="66" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
-      <c r="E4" s="69"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="68"/>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="69"/>
-      <c r="C5" s="70"/>
-      <c r="E5" s="69"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="68"/>
+      <c r="E5" s="67"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="70"/>
+      <c r="C6" s="68"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="70"/>
+      <c r="C7" s="68"/>
     </row>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>